<commit_message>
add openstack content into lqbz.xlsx
</commit_message>
<xml_diff>
--- a/lqbz.xlsx
+++ b/lqbz.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="312">
   <si>
     <t>http://www.open-open.com/lib/view/open1460134175743.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1313,6 +1313,14 @@
   </si>
   <si>
     <t>9、WWN信息搜索 - 前端</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.csdn.net/u011521019/article/details/51301672</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openstack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1701,6 +1709,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1713,6 +1724,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1725,51 +1781,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1784,9 +1795,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2085,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2219,6 +2227,16 @@
         <v>245</v>
       </c>
     </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
     <row r="24" spans="1:3">
       <c r="C24" t="s">
         <v>276</v>
@@ -2271,9 +2289,10 @@
     <hyperlink ref="A5" r:id="rId3"/>
     <hyperlink ref="C6" r:id="rId4"/>
     <hyperlink ref="C25" r:id="rId5"/>
+    <hyperlink ref="A23" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2302,30 +2321,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="16"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" ht="16.5">
       <c r="A2" s="2" t="s">
@@ -2760,10 +2779,10 @@
       <c r="J13" t="s">
         <v>166</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="13"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="16.5">
       <c r="C14" s="2" t="s">
@@ -3065,10 +3084,10 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="3:12">
-      <c r="K31" s="13" t="s">
+      <c r="K31" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="13"/>
+      <c r="L31" s="14"/>
     </row>
     <row r="32" spans="3:12" ht="16.5">
       <c r="K32" s="2" t="s">
@@ -3143,92 +3162,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="93.75" customHeight="1" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="29"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="29"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="7" t="s">
         <v>263</v>
       </c>
@@ -3237,92 +3256,87 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="24" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="22"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="27"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="29"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="33" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="30" t="s">
         <v>269</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="25"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="22"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="27"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="22"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A16" s="23"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="29"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:C16"/>
-    <mergeCell ref="D13:F16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:B8"/>
@@ -3338,6 +3352,11 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="D6:F7"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:C16"/>
+    <mergeCell ref="D13:F16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3366,7 +3385,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="40">
+      <c r="A2" s="41">
         <v>2017</v>
       </c>
       <c r="B2" s="11">
@@ -3374,181 +3393,181 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="40"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="11">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="11">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="40"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="11">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="11">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="11">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="11">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="12">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="40"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="12">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="11">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="40"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="12">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="40"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="40"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="11">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="11">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="40"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="11">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="40"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="11">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="40"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="11">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="40"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="11">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="40"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="11">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="40"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="11">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="40"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="40"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="11">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="40"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="11">
         <v>31</v>
       </c>
@@ -3567,8 +3586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3645,24 +3664,24 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="13" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="13" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
up lqbz.xlsx and delete anlulu
</commit_message>
<xml_diff>
--- a/lqbz.xlsx
+++ b/lqbz.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="368">
   <si>
     <t>http://www.open-open.com/lib/view/open1460134175743.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1252,10 +1252,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>进行中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://blog.csdn.net/u011521019/article/details/51301672</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1276,10 +1272,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>进行中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>已完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1297,12 +1289,6 @@
     <t>查看设备ZONE前端页面</t>
   </si>
   <si>
-    <t>在线选课系统</t>
-  </si>
-  <si>
-    <t>服务器管理系统</t>
-  </si>
-  <si>
     <t>第一阶段</t>
   </si>
   <si>
@@ -1417,10 +1403,6 @@
   </si>
   <si>
     <t>完成时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>---------</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1537,6 +1519,35 @@
     <t>1、san存储自服务页面编写
 2、讨论san存储自服务系统流程具体需求</t>
     <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、服务器管理系统页面修改
+2、划zone自服务页面编写</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、划zone自服务页面编写和调整</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>第十九阶段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在线选课系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器管理系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>划zone自服务页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1677,7 +1688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1937,6 +1948,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1947,7 +1971,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2026,6 +2050,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2038,51 +2107,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2121,6 +2145,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2553,12 +2580,12 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3486,92 +3513,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="93.75" customHeight="1" thickBot="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="42" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>255</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>256</v>
       </c>
       <c r="C4" s="46"/>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A5" s="32"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="47"/>
       <c r="C5" s="48"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="38"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>258</v>
       </c>
       <c r="B6" s="45" t="s">
         <v>259</v>
       </c>
       <c r="C6" s="46"/>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A7" s="32"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="47"/>
       <c r="C7" s="48"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="38"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="7" t="s">
         <v>263</v>
       </c>
@@ -3580,92 +3607,87 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="31"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="36"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="38"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="42" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="44"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="33" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="36"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="36"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A16" s="32"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="38"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:C16"/>
-    <mergeCell ref="D13:F16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:B8"/>
@@ -3681,6 +3703,11 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="D6:F7"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:C16"/>
+    <mergeCell ref="D13:F16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3693,7 +3720,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3708,16 +3735,16 @@
         <v>291</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>298</v>
-      </c>
       <c r="E1" s="11" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>343</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4006,7 +4033,7 @@
       <c r="E17" s="11">
         <v>16</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="12">
         <v>16</v>
       </c>
     </row>
@@ -4024,7 +4051,7 @@
       <c r="E18" s="12">
         <v>17</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="12">
         <v>17</v>
       </c>
     </row>
@@ -4042,7 +4069,7 @@
       <c r="E19" s="11">
         <v>18</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="12">
         <v>18</v>
       </c>
     </row>
@@ -4060,7 +4087,7 @@
       <c r="E20" s="11">
         <v>19</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="12">
         <v>19</v>
       </c>
     </row>
@@ -4284,10 +4311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4300,24 +4327,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C2" s="14">
         <v>42649</v>
@@ -4328,10 +4355,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C3" s="14">
         <v>42666</v>
@@ -4342,10 +4369,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C4" s="14">
         <v>42679</v>
@@ -4356,10 +4383,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C5" s="14">
         <v>42705</v>
@@ -4370,10 +4397,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C6" s="14">
         <v>42719</v>
@@ -4384,36 +4411,36 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C7" s="14">
         <v>42809</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="13" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C9" s="14">
         <v>42755</v>
@@ -4424,10 +4451,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C10" s="14">
         <v>42760</v>
@@ -4438,24 +4465,24 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C11" s="14">
         <v>42755</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C12" s="14">
         <v>42750</v>
@@ -4466,10 +4493,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C13" s="14">
         <v>42789</v>
@@ -4480,10 +4507,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C14" s="14">
         <v>42804</v>
@@ -4494,10 +4521,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C15" s="14">
         <v>42814</v>
@@ -4507,25 +4534,25 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>299</v>
+      <c r="A16" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C16" s="14">
+        <v>42859</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C17" s="14">
         <v>42830</v>
@@ -4535,30 +4562,44 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>293</v>
+      <c r="A18" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C18" s="14">
+        <v>42860</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C19" s="14">
         <v>42832</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="C20" s="14">
+        <v>42877</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>292</v>
       </c>
     </row>
@@ -4571,10 +4612,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4586,20 +4627,20 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="51" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="18" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="38.25" customHeight="1">
@@ -4607,10 +4648,10 @@
         <v>4.12</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="48" customHeight="1">
@@ -4618,7 +4659,7 @@
         <v>4.13</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C4" s="54"/>
     </row>
@@ -4627,26 +4668,26 @@
         <v>4.1399999999999997</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C5" s="55"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="50" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="18" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="36.75" customHeight="1">
@@ -4654,28 +4695,28 @@
         <v>4.17</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="50" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="18" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="33" customHeight="1">
@@ -4683,10 +4724,10 @@
         <v>4.26</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" customHeight="1">
@@ -4694,26 +4735,26 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C16" s="57"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="50" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="18" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="33" customHeight="1">
@@ -4721,7 +4762,7 @@
         <v>5.2</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C21" s="21"/>
     </row>
@@ -4730,7 +4771,7 @@
         <v>5.3</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C22" s="21"/>
     </row>
@@ -4739,26 +4780,26 @@
         <v>5.4</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C23" s="21"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="50" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="18" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="38.25" customHeight="1">
@@ -4766,7 +4807,7 @@
         <v>5.9</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C28" s="21"/>
     </row>
@@ -4775,7 +4816,7 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C29" s="21"/>
     </row>
@@ -4784,12 +4825,64 @@
         <v>5.12</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C30" s="21"/>
     </row>
+    <row r="33" spans="1:3" ht="18" customHeight="1">
+      <c r="A33" s="50" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" customHeight="1">
+      <c r="A35" s="19">
+        <v>5.16</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="19">
+        <v>5.17</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>362</v>
+      </c>
+      <c r="C36" s="58"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="19">
+        <v>5.18</v>
+      </c>
+      <c r="B37" s="54"/>
+      <c r="C37" s="58"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="19">
+        <v>5.19</v>
+      </c>
+      <c r="B38" s="55"/>
+      <c r="C38" s="58"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   lqbz.xlsx
</commit_message>
<xml_diff>
--- a/lqbz.xlsx
+++ b/lqbz.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2038,6 +2038,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2050,6 +2053,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2089,24 +2104,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2125,6 +2128,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2132,22 +2144,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2672,30 +2672,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="24"/>
+      <c r="G1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="25" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="25"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="16.5">
       <c r="A2" s="2" t="s">
@@ -3130,10 +3130,10 @@
       <c r="J13" t="s">
         <v>166</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="22"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" ht="16.5">
       <c r="C14" s="2" t="s">
@@ -3435,10 +3435,10 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="3:12">
-      <c r="K31" s="22" t="s">
+      <c r="K31" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="22"/>
+      <c r="L31" s="23"/>
     </row>
     <row r="32" spans="3:12" ht="16.5">
       <c r="K32" s="2" t="s">
@@ -3513,92 +3513,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" ht="93.75" customHeight="1" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="38" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="34"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="30"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="34"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="43" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="7" t="s">
         <v>263</v>
       </c>
@@ -3607,87 +3607,92 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="29" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="27"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="32"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A11" s="28"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="34"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="43" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="38" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="43" t="s">
         <v>269</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="27"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="32"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="27"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="32"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" thickBot="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="34"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:C16"/>
+    <mergeCell ref="D13:F16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:B8"/>
@@ -3703,11 +3708,6 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:C7"/>
     <mergeCell ref="D6:F7"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:C16"/>
-    <mergeCell ref="D13:F16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3719,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3748,7 +3748,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="49">
+      <c r="A2" s="50">
         <v>2017</v>
       </c>
       <c r="B2" s="11">
@@ -3768,7 +3768,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="49"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="11">
         <v>2</v>
       </c>
@@ -3786,7 +3786,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="49"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="11">
         <v>3</v>
       </c>
@@ -3804,7 +3804,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="49"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="11">
         <v>4</v>
       </c>
@@ -3822,7 +3822,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="12">
         <v>5</v>
       </c>
@@ -3840,7 +3840,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="49"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="11">
         <v>6</v>
       </c>
@@ -3858,7 +3858,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="49"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="11">
         <v>7</v>
       </c>
@@ -3876,7 +3876,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="11">
         <v>8</v>
       </c>
@@ -3894,7 +3894,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="11">
         <v>9</v>
       </c>
@@ -3912,7 +3912,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="49"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="12">
         <v>10</v>
       </c>
@@ -3930,7 +3930,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="11">
         <v>11</v>
       </c>
@@ -3948,7 +3948,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="12">
         <v>12</v>
       </c>
@@ -3966,7 +3966,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="11">
         <v>13</v>
       </c>
@@ -3984,7 +3984,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="11">
         <v>14</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="11">
         <v>15</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="12">
         <v>16</v>
       </c>
@@ -4038,7 +4038,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="49"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="12">
         <v>17</v>
       </c>
@@ -4056,7 +4056,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="11">
         <v>18</v>
       </c>
@@ -4074,7 +4074,7 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="12">
         <v>19</v>
       </c>
@@ -4092,7 +4092,7 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="11">
         <v>20</v>
       </c>
@@ -4110,7 +4110,7 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="11">
         <v>21</v>
       </c>
@@ -4128,7 +4128,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="49"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="11">
         <v>22</v>
       </c>
@@ -4146,7 +4146,7 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="11">
         <v>23</v>
       </c>
@@ -4159,12 +4159,12 @@
       <c r="E24" s="11">
         <v>23</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="12">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="11">
         <v>24</v>
       </c>
@@ -4182,7 +4182,7 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="11">
         <v>25</v>
       </c>
@@ -4200,7 +4200,7 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="11">
         <v>26</v>
       </c>
@@ -4213,12 +4213,12 @@
       <c r="E27" s="12">
         <v>26</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="12">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="11">
         <v>27</v>
       </c>
@@ -4231,12 +4231,12 @@
       <c r="E28" s="12">
         <v>27</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="12">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="49"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="11">
         <v>28</v>
       </c>
@@ -4254,7 +4254,7 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="11">
         <v>29</v>
       </c>
@@ -4270,7 +4270,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="49"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="11">
         <v>30</v>
       </c>
@@ -4286,7 +4286,7 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="49"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="11">
         <v>31</v>
       </c>
@@ -4614,7 +4614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -4626,11 +4626,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>339</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="18" t="s">
@@ -4650,7 +4650,7 @@
       <c r="B3" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>344</v>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
       <c r="B4" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="53"/>
     </row>
     <row r="5" spans="1:3" ht="46.5" customHeight="1">
       <c r="A5" s="19">
@@ -4670,14 +4670,14 @@
       <c r="B5" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="54"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="18" t="s">
@@ -4702,11 +4702,11 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="18" t="s">
@@ -4726,7 +4726,7 @@
       <c r="B15" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="57" t="s">
         <v>351</v>
       </c>
     </row>
@@ -4737,14 +4737,14 @@
       <c r="B16" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="C16" s="57"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="51" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="18" t="s">
@@ -4785,11 +4785,11 @@
       <c r="C23" s="21"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="51" t="s">
         <v>352</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="18" t="s">
@@ -4830,11 +4830,11 @@
       <c r="C30" s="21"/>
     </row>
     <row r="33" spans="1:3" ht="18" customHeight="1">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="51" t="s">
         <v>352</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
       <c r="A34" s="18" t="s">
@@ -4860,24 +4860,24 @@
       <c r="A36" s="19">
         <v>5.17</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="52" t="s">
         <v>362</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="22"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="19">
         <v>5.18</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="58"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="22"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="19">
         <v>5.19</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="58"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>